<commit_message>
add major_good to stock
</commit_message>
<xml_diff>
--- a/database/industries/siman/save/official/quarterly.xlsx
+++ b/database/industries/siman/save/official/quarterly.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\siman\save\official\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\siman\save\official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75943B6B-421E-417B-A414-51434C600D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="2748" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="2745" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -34,9 +33,6 @@
     <t>هزینه های عمومی و اداری</t>
   </si>
   <si>
-    <t>فصل دوم منتهی به 1400/06</t>
-  </si>
-  <si>
     <t>فصل سوم منتهی به 1400/09</t>
   </si>
   <si>
@@ -89,13 +85,20 @@
   </si>
   <si>
     <t>تعداد پرسنل تولیدی شرکت</t>
+  </si>
+  <si>
+    <t>فصل سوم منتهی به 1401/09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
@@ -124,6 +127,11 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri Bold"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -186,10 +194,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -224,8 +233,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,17 +551,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="20" customWidth="1"/>
+    <col min="2" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -555,9 +572,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,9 +583,8 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -579,9 +594,8 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -589,9 +603,8 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="2:9" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    </row>
+    <row r="5" spans="2:9" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -601,9 +614,8 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="2:9" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    </row>
+    <row r="6" spans="2:9" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -613,9 +625,8 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -623,9 +634,8 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="2:9" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
@@ -644,10 +654,10 @@
         <v>7</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -655,11 +665,10 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -673,15 +682,15 @@
         <v>0</v>
       </c>
       <c r="H10" s="9">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
         <v>142896</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="14">
+        <v>664256</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -697,13 +706,13 @@
       <c r="H11" s="11">
         <v>0</v>
       </c>
-      <c r="I11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -716,38 +725,38 @@
       <c r="G12" s="9">
         <v>0</v>
       </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11">
-        <v>2737</v>
+        <v>-2915</v>
       </c>
       <c r="F13" s="11">
-        <v>-2915</v>
+        <v>1292</v>
       </c>
       <c r="G13" s="11">
-        <v>1292</v>
+        <v>30</v>
       </c>
       <c r="H13" s="11">
-        <v>30</v>
-      </c>
-      <c r="I13" s="11">
         <v>290</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="15">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -763,79 +772,79 @@
       <c r="H14" s="9">
         <v>0</v>
       </c>
-      <c r="I14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11">
-        <v>-82</v>
+        <v>523</v>
       </c>
       <c r="F15" s="11">
-        <v>523</v>
+        <v>173</v>
       </c>
       <c r="G15" s="11">
-        <v>173</v>
+        <v>13</v>
       </c>
       <c r="H15" s="11">
-        <v>13</v>
-      </c>
-      <c r="I15" s="11">
         <v>8768</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="15">
+        <v>-8671</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9">
-        <v>703</v>
+        <v>764</v>
       </c>
       <c r="F16" s="9">
-        <v>764</v>
+        <v>975</v>
       </c>
       <c r="G16" s="9">
-        <v>975</v>
+        <v>786</v>
       </c>
       <c r="H16" s="9">
-        <v>786</v>
-      </c>
-      <c r="I16" s="9">
         <v>2500</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I16" s="15">
+        <v>3672</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11">
-        <v>20568</v>
+        <v>20034</v>
       </c>
       <c r="F17" s="11">
-        <v>20034</v>
+        <v>20039</v>
       </c>
       <c r="G17" s="11">
-        <v>20039</v>
+        <v>42258</v>
       </c>
       <c r="H17" s="11">
-        <v>42258</v>
-      </c>
-      <c r="I17" s="11">
         <v>41113</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="15">
+        <v>30341</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -851,55 +860,56 @@
       <c r="H18" s="9">
         <v>0</v>
       </c>
-      <c r="I18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11">
-        <v>166230</v>
+        <v>75670</v>
       </c>
       <c r="F19" s="11">
-        <v>75670</v>
+        <v>136214</v>
       </c>
       <c r="G19" s="11">
-        <v>136214</v>
+        <v>104716</v>
       </c>
       <c r="H19" s="11">
-        <v>104716</v>
-      </c>
-      <c r="I19" s="11">
         <v>-7835</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="15">
+        <v>19440</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13">
-        <v>190156</v>
+        <v>94076</v>
       </c>
       <c r="F20" s="13">
-        <v>94076</v>
+        <v>158693</v>
       </c>
       <c r="G20" s="13">
-        <v>158693</v>
+        <v>147803</v>
       </c>
       <c r="H20" s="13">
-        <v>147803</v>
-      </c>
-      <c r="I20" s="13">
         <v>187732</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="14">
+        <f>SUM(I10:I19)</f>
+        <v>709440</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -907,9 +917,8 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -917,9 +926,8 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -927,11 +935,10 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="2:9" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -948,10 +955,10 @@
         <v>7</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -959,53 +966,52 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9">
-        <v>71</v>
+        <v>410</v>
       </c>
       <c r="F26" s="9">
-        <v>410</v>
+        <v>551</v>
       </c>
       <c r="G26" s="9">
-        <v>551</v>
+        <v>629</v>
       </c>
       <c r="H26" s="9">
-        <v>629</v>
+        <v>574</v>
       </c>
       <c r="I26" s="9">
         <v>574</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11">
-        <v>406</v>
+        <v>66</v>
       </c>
       <c r="F27" s="11">
+        <v>144</v>
+      </c>
+      <c r="G27" s="11">
         <v>66</v>
       </c>
-      <c r="G27" s="11">
-        <v>144</v>
-      </c>
       <c r="H27" s="11">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="I27" s="11">
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1013,9 +1019,8 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1023,9 +1028,8 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1033,9 +1037,8 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1043,7 +1046,6 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>